<commit_message>
docs: add some notes to Rekapitulasi_Hasil_SKD_Jabatan_Manggala_Informatika_Kemkominfo_CPNS_2024.xlsx
</commit_message>
<xml_diff>
--- a/data/other/Rekapitulasi_Hasil_SKD_Jabatan_Manggala_Informatika_Kemkominfo_CPNS_2024.xlsx
+++ b/data/other/Rekapitulasi_Hasil_SKD_Jabatan_Manggala_Informatika_Kemkominfo_CPNS_2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\1. Career\1. CPNS 2024\1. SKD\5. Rekapitulasi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waskito\project\github\waskitof\me\data\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BBBF13-8E23-452B-9F0D-3619031CAEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72BA594-CDE0-4835-B332-99AD31E15E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{6A330717-C359-4640-9D6E-86922AF56F0F}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="215">
   <si>
     <t>TWK</t>
   </si>
@@ -706,9 +706,6 @@
     <t>Tidak memenuhi nilai ambang batas SKD</t>
   </si>
   <si>
-    <t>DISTRIBUSI STATUS HASIL SKD JABATAN MANGGALA INFORMATIKA KEMKOMINFO DI SELURUH UNIT KERJA KEMKOMINFO CPNS 2024</t>
-  </si>
-  <si>
     <t>NILAI AMBANG BATAS</t>
   </si>
   <si>
@@ -897,6 +894,181 @@
       <t xml:space="preserve"> (Nomor 6 Tahun 2024).</t>
     </r>
   </si>
+  <si>
+    <t>DISTRIBUSI STATUS HASIL SKD JABATAN MANGGALA INFORMATIKA DI SELURUH UNIT KERJA KEMKOMINFO CPNS 2024</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mengingat keterbatasn informasi, setiap peserta dianggap melamar kategori </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CPNS Umum</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Meskipun, terdapat sejumlah 2 kebutuhan untuk kategori </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CPNS Putra/Putri Kalimantan</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Perankingan peserta</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> di sini di lakukan secara </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nasional</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Meskipun, perankingan sesungguhnya akan dilakukan per </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>penempatan</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unit kerja)</t>
+    </r>
+  </si>
+  <si>
+    <t>https://jdih.menpan.go.id/common/dokumen/2024kepmenpanrb321.pdf</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kementerian Pendayagunaan Aparatur Negara dan Reformasi Birokrasi. (2024). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Peraturan meteri pendayagunaan aparatur negara dan reformasi birokrasi republik Indonesia: Nilai ambang batas seleksi kompetensi dasar pengadaan pegawai negeri sipil tahun anggaran 2024</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Nomor 321 Tahun 2024).</t>
+    </r>
+  </si>
+  <si>
+    <t>Rekapitulasi dilakukan melalui pencocokan data pada lampiran pengumuman peserta lolos administrasi pasca sanggah dan jadwal SKD terhadap live score bersangkutan. Jadi, tidak menutup kemungkinan bahwa rekapitulasi ini memuat kekeliruan di dalamnya.</t>
+  </si>
+  <si>
+    <t>Rekapitulasi ini sejatinya milik personal, tetapi kemudian dibagikan semata-mata dalam rangka berbagi informasi bagi sesama dan tidak ada maksud lain di baliknya.</t>
+  </si>
 </sst>
 </file>
 
@@ -905,7 +1077,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1085,6 +1257,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -1178,7 +1358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1365,12 +1545,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1725,8 +1914,41 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1806,29 +2028,12 @@
     <xf numFmtId="0" fontId="16" fillId="15" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4180,23 +4385,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="134" t="s">
-        <v>190</v>
-      </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="134"/>
-      <c r="O2" s="134"/>
+      <c r="A2" s="144" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="M2" s="144"/>
+      <c r="N2" s="144"/>
+      <c r="O2" s="144"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -4210,21 +4415,21 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="134"/>
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
-      <c r="K3" s="134"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="134"/>
-      <c r="N3" s="134"/>
-      <c r="O3" s="134"/>
+      <c r="A3" s="144"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
+      <c r="O3" s="144"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -4621,15 +4826,17 @@
       <c r="G14" s="122">
         <v>1</v>
       </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
+      <c r="H14" s="146" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="147"/>
+      <c r="J14" s="142"/>
+      <c r="K14" s="142"/>
+      <c r="L14" s="142"/>
+      <c r="M14" s="142"/>
+      <c r="N14" s="142"/>
+      <c r="O14" s="142"/>
+      <c r="P14" s="142"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
@@ -4655,15 +4862,19 @@
       <c r="G15" s="122">
         <v>1</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
+      <c r="H15" s="143" t="s">
+        <v>209</v>
+      </c>
+      <c r="I15" s="145" t="s">
+        <v>208</v>
+      </c>
+      <c r="J15" s="145"/>
+      <c r="K15" s="145"/>
+      <c r="L15" s="145"/>
+      <c r="M15" s="145"/>
+      <c r="N15" s="145"/>
+      <c r="O15" s="145"/>
+      <c r="P15" s="145"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
@@ -4692,14 +4903,14 @@
         <v>2</v>
       </c>
       <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+      <c r="I16" s="145"/>
+      <c r="J16" s="145"/>
+      <c r="K16" s="145"/>
+      <c r="L16" s="145"/>
+      <c r="M16" s="145"/>
+      <c r="N16" s="145"/>
+      <c r="O16" s="145"/>
+      <c r="P16" s="145"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
@@ -4725,15 +4936,19 @@
       <c r="G17" s="122">
         <v>4</v>
       </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
+      <c r="H17" s="143" t="s">
+        <v>209</v>
+      </c>
+      <c r="I17" s="145" t="s">
+        <v>210</v>
+      </c>
+      <c r="J17" s="145"/>
+      <c r="K17" s="145"/>
+      <c r="L17" s="145"/>
+      <c r="M17" s="145"/>
+      <c r="N17" s="145"/>
+      <c r="O17" s="145"/>
+      <c r="P17" s="145"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
@@ -4764,14 +4979,14 @@
         <v>4</v>
       </c>
       <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
+      <c r="I18" s="145"/>
+      <c r="J18" s="145"/>
+      <c r="K18" s="145"/>
+      <c r="L18" s="145"/>
+      <c r="M18" s="145"/>
+      <c r="N18" s="145"/>
+      <c r="O18" s="145"/>
+      <c r="P18" s="145"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
@@ -4783,7 +4998,7 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="121" t="s">
         <v>21</v>
       </c>
@@ -4797,15 +5012,19 @@
       <c r="G19" s="122">
         <v>1</v>
       </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
+      <c r="H19" s="143" t="s">
+        <v>209</v>
+      </c>
+      <c r="I19" s="145" t="s">
+        <v>213</v>
+      </c>
+      <c r="J19" s="145"/>
+      <c r="K19" s="145"/>
+      <c r="L19" s="145"/>
+      <c r="M19" s="145"/>
+      <c r="N19" s="145"/>
+      <c r="O19" s="145"/>
+      <c r="P19" s="145"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
@@ -4832,14 +5051,14 @@
         <v>1</v>
       </c>
       <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
+      <c r="I20" s="145"/>
+      <c r="J20" s="145"/>
+      <c r="K20" s="145"/>
+      <c r="L20" s="145"/>
+      <c r="M20" s="145"/>
+      <c r="N20" s="145"/>
+      <c r="O20" s="145"/>
+      <c r="P20" s="145"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
@@ -4851,7 +5070,7 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="121" t="s">
         <v>30</v>
       </c>
@@ -4866,14 +5085,14 @@
         <v>2</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
+      <c r="I21" s="145"/>
+      <c r="J21" s="145"/>
+      <c r="K21" s="145"/>
+      <c r="L21" s="145"/>
+      <c r="M21" s="145"/>
+      <c r="N21" s="145"/>
+      <c r="O21" s="145"/>
+      <c r="P21" s="145"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
@@ -4901,15 +5120,19 @@
       <c r="G22" s="122">
         <v>3</v>
       </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
+      <c r="H22" s="143" t="s">
+        <v>209</v>
+      </c>
+      <c r="I22" s="145" t="s">
+        <v>214</v>
+      </c>
+      <c r="J22" s="145"/>
+      <c r="K22" s="145"/>
+      <c r="L22" s="145"/>
+      <c r="M22" s="145"/>
+      <c r="N22" s="145"/>
+      <c r="O22" s="145"/>
+      <c r="P22" s="145"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
@@ -4921,7 +5144,7 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="121" t="s">
         <v>31</v>
       </c>
@@ -4936,14 +5159,14 @@
         <v>1</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
+      <c r="I23" s="145"/>
+      <c r="J23" s="145"/>
+      <c r="K23" s="145"/>
+      <c r="L23" s="145"/>
+      <c r="M23" s="145"/>
+      <c r="N23" s="145"/>
+      <c r="O23" s="145"/>
+      <c r="P23" s="145"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
@@ -4972,14 +5195,14 @@
         <v>2</v>
       </c>
       <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
+      <c r="I24" s="175"/>
+      <c r="J24" s="175"/>
+      <c r="K24" s="175"/>
+      <c r="L24" s="175"/>
+      <c r="M24" s="175"/>
+      <c r="N24" s="175"/>
+      <c r="O24" s="175"/>
+      <c r="P24" s="175"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
@@ -7150,8 +7373,13 @@
       <c r="Z100" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="I22:P23"/>
+    <mergeCell ref="I19:P21"/>
     <mergeCell ref="A2:O3"/>
+    <mergeCell ref="I15:P16"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="I17:P18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -7240,24 +7468,24 @@
       <c r="AD1" s="12"/>
     </row>
     <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="144" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="134"/>
-      <c r="O2" s="134"/>
-      <c r="P2" s="134"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="M2" s="144"/>
+      <c r="N2" s="144"/>
+      <c r="O2" s="144"/>
+      <c r="P2" s="144"/>
       <c r="Q2" s="38"/>
       <c r="R2" s="38"/>
       <c r="S2" s="38"/>
@@ -7274,22 +7502,22 @@
       <c r="AD2" s="12"/>
     </row>
     <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="134"/>
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
-      <c r="K3" s="134"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="134"/>
-      <c r="N3" s="134"/>
-      <c r="O3" s="134"/>
-      <c r="P3" s="134"/>
+      <c r="A3" s="144"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
+      <c r="O3" s="144"/>
+      <c r="P3" s="144"/>
       <c r="Q3" s="38"/>
       <c r="R3" s="38"/>
       <c r="S3" s="38"/>
@@ -7373,27 +7601,27 @@
       <c r="A6" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="152" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="140"/>
-      <c r="D6" s="141"/>
-      <c r="E6" s="142" t="s">
+      <c r="C6" s="153"/>
+      <c r="D6" s="154"/>
+      <c r="E6" s="155" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="144"/>
+      <c r="F6" s="156"/>
+      <c r="G6" s="156"/>
+      <c r="H6" s="157"/>
       <c r="I6" s="51"/>
       <c r="J6" s="26"/>
       <c r="K6" s="40"/>
-      <c r="L6" s="145"/>
-      <c r="M6" s="145"/>
-      <c r="N6" s="145"/>
-      <c r="O6" s="145"/>
-      <c r="P6" s="145"/>
-      <c r="Q6" s="145"/>
-      <c r="R6" s="145"/>
+      <c r="L6" s="158"/>
+      <c r="M6" s="158"/>
+      <c r="N6" s="158"/>
+      <c r="O6" s="158"/>
+      <c r="P6" s="158"/>
+      <c r="Q6" s="158"/>
+      <c r="R6" s="158"/>
       <c r="S6" s="41"/>
       <c r="T6" s="14"/>
       <c r="U6" s="14"/>
@@ -7436,12 +7664,12 @@
         <v>40</v>
       </c>
       <c r="J7" s="27"/>
-      <c r="K7" s="148" t="s">
+      <c r="K7" s="161" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="149"/>
-      <c r="M7" s="149"/>
-      <c r="N7" s="149"/>
+      <c r="L7" s="162"/>
+      <c r="M7" s="162"/>
+      <c r="N7" s="162"/>
       <c r="O7" s="86" t="s">
         <v>42</v>
       </c>
@@ -7493,12 +7721,12 @@
         <v>32</v>
       </c>
       <c r="J8" s="28"/>
-      <c r="K8" s="152" t="s">
+      <c r="K8" s="165" t="s">
         <v>184</v>
       </c>
-      <c r="L8" s="153"/>
-      <c r="M8" s="153"/>
-      <c r="N8" s="153"/>
+      <c r="L8" s="166"/>
+      <c r="M8" s="166"/>
+      <c r="N8" s="166"/>
       <c r="O8" s="50">
         <f>COUNTIF($I$8:$I$120,"P")</f>
         <v>77</v>
@@ -7552,12 +7780,12 @@
         <v>182</v>
       </c>
       <c r="J9" s="28"/>
-      <c r="K9" s="152" t="s">
+      <c r="K9" s="165" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="153"/>
-      <c r="M9" s="153"/>
-      <c r="N9" s="153"/>
+      <c r="L9" s="166"/>
+      <c r="M9" s="166"/>
+      <c r="N9" s="166"/>
       <c r="O9" s="50">
         <f>COUNTIF($I$8:$I$120,"PS")</f>
         <v>1</v>
@@ -7611,12 +7839,12 @@
         <v>32</v>
       </c>
       <c r="J10" s="28"/>
-      <c r="K10" s="152" t="s">
+      <c r="K10" s="165" t="s">
         <v>51</v>
       </c>
-      <c r="L10" s="153"/>
-      <c r="M10" s="153"/>
-      <c r="N10" s="153"/>
+      <c r="L10" s="166"/>
+      <c r="M10" s="166"/>
+      <c r="N10" s="166"/>
       <c r="O10" s="50">
         <f>COUNTIF($I$8:$I$120,"TD")</f>
         <v>2</v>
@@ -7670,12 +7898,12 @@
         <v>32</v>
       </c>
       <c r="J11" s="28"/>
-      <c r="K11" s="152" t="s">
-        <v>194</v>
-      </c>
-      <c r="L11" s="153"/>
-      <c r="M11" s="153"/>
-      <c r="N11" s="153"/>
+      <c r="K11" s="165" t="s">
+        <v>193</v>
+      </c>
+      <c r="L11" s="166"/>
+      <c r="M11" s="166"/>
+      <c r="N11" s="166"/>
       <c r="O11" s="50">
         <f>COUNTIF($I$8:$I$120,"TH")</f>
         <v>9</v>
@@ -7729,12 +7957,12 @@
         <v>182</v>
       </c>
       <c r="J12" s="28"/>
-      <c r="K12" s="152" t="s">
+      <c r="K12" s="165" t="s">
         <v>185</v>
       </c>
-      <c r="L12" s="153"/>
-      <c r="M12" s="153"/>
-      <c r="N12" s="153"/>
+      <c r="L12" s="166"/>
+      <c r="M12" s="166"/>
+      <c r="N12" s="166"/>
       <c r="O12" s="50">
         <f>COUNTIF($I$8:$I$120,"TL")</f>
         <v>24</v>
@@ -7788,12 +8016,12 @@
         <v>32</v>
       </c>
       <c r="J13" s="28"/>
-      <c r="K13" s="150" t="s">
+      <c r="K13" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="151"/>
-      <c r="M13" s="151"/>
-      <c r="N13" s="151"/>
+      <c r="L13" s="164"/>
+      <c r="M13" s="164"/>
+      <c r="N13" s="164"/>
       <c r="O13" s="93">
         <f>SUM(O8:O12)</f>
         <v>113</v>
@@ -7949,12 +8177,12 @@
         <v>32</v>
       </c>
       <c r="J16" s="28"/>
-      <c r="K16" s="146" t="s">
+      <c r="K16" s="159" t="s">
         <v>37</v>
       </c>
-      <c r="L16" s="147"/>
-      <c r="M16" s="147"/>
-      <c r="N16" s="147"/>
+      <c r="L16" s="160"/>
+      <c r="M16" s="160"/>
+      <c r="N16" s="160"/>
       <c r="O16" s="91" t="s">
         <v>42</v>
       </c>
@@ -8006,12 +8234,12 @@
         <v>32</v>
       </c>
       <c r="J17" s="28"/>
-      <c r="K17" s="135" t="s">
+      <c r="K17" s="148" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="136"/>
-      <c r="M17" s="136"/>
-      <c r="N17" s="136"/>
+      <c r="L17" s="149"/>
+      <c r="M17" s="149"/>
+      <c r="N17" s="149"/>
       <c r="O17" s="74">
         <f>COUNTIF($B$8:$B$120,"Aceh 2")</f>
         <v>1</v>
@@ -8065,12 +8293,12 @@
         <v>32</v>
       </c>
       <c r="J18" s="28"/>
-      <c r="K18" s="135" t="s">
+      <c r="K18" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="L18" s="136"/>
-      <c r="M18" s="136"/>
-      <c r="N18" s="136"/>
+      <c r="L18" s="149"/>
+      <c r="M18" s="149"/>
+      <c r="N18" s="149"/>
       <c r="O18" s="74">
         <f>COUNTIF($B$8:$B$120,"Aceh Timur")</f>
         <v>1</v>
@@ -8115,12 +8343,12 @@
         <v>183</v>
       </c>
       <c r="J19" s="28"/>
-      <c r="K19" s="135" t="s">
+      <c r="K19" s="148" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="136"/>
-      <c r="M19" s="136"/>
-      <c r="N19" s="136"/>
+      <c r="L19" s="149"/>
+      <c r="M19" s="149"/>
+      <c r="N19" s="149"/>
       <c r="O19" s="74">
         <f>COUNTIF($B$8:$B$120,"Aula Univ. Bojonegoro")</f>
         <v>1</v>
@@ -8165,12 +8393,12 @@
         <v>183</v>
       </c>
       <c r="J20" s="28"/>
-      <c r="K20" s="135" t="s">
+      <c r="K20" s="148" t="s">
         <v>7</v>
       </c>
-      <c r="L20" s="136"/>
-      <c r="M20" s="136"/>
-      <c r="N20" s="136"/>
+      <c r="L20" s="149"/>
+      <c r="M20" s="149"/>
+      <c r="N20" s="149"/>
       <c r="O20" s="74">
         <f>COUNTIF($B$8:$B$120,"Bandung 1")</f>
         <v>8</v>
@@ -8224,12 +8452,12 @@
         <v>32</v>
       </c>
       <c r="J21" s="28"/>
-      <c r="K21" s="135" t="s">
+      <c r="K21" s="148" t="s">
         <v>29</v>
       </c>
-      <c r="L21" s="136"/>
-      <c r="M21" s="136"/>
-      <c r="N21" s="136"/>
+      <c r="L21" s="149"/>
+      <c r="M21" s="149"/>
+      <c r="N21" s="149"/>
       <c r="O21" s="74">
         <f>COUNTIF($B$8:$B$120,"Batam")</f>
         <v>2</v>
@@ -8283,12 +8511,12 @@
         <v>182</v>
       </c>
       <c r="J22" s="28"/>
-      <c r="K22" s="135" t="s">
+      <c r="K22" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="L22" s="136"/>
-      <c r="M22" s="136"/>
-      <c r="N22" s="136"/>
+      <c r="L22" s="149"/>
+      <c r="M22" s="149"/>
+      <c r="N22" s="149"/>
       <c r="O22" s="74">
         <f>COUNTIF($B$8:$B$120,"IC Malang")</f>
         <v>5</v>
@@ -8342,12 +8570,12 @@
         <v>32</v>
       </c>
       <c r="J23" s="28"/>
-      <c r="K23" s="135" t="s">
+      <c r="K23" s="148" t="s">
         <v>4</v>
       </c>
-      <c r="L23" s="136"/>
-      <c r="M23" s="136"/>
-      <c r="N23" s="136"/>
+      <c r="L23" s="149"/>
+      <c r="M23" s="149"/>
+      <c r="N23" s="149"/>
       <c r="O23" s="74">
         <f>COUNTIF($B$8:$B$120,"Jakarta 2")</f>
         <v>58</v>
@@ -8401,12 +8629,12 @@
         <v>182</v>
       </c>
       <c r="J24" s="28"/>
-      <c r="K24" s="135" t="s">
+      <c r="K24" s="148" t="s">
         <v>25</v>
       </c>
-      <c r="L24" s="136"/>
-      <c r="M24" s="136"/>
-      <c r="N24" s="136"/>
+      <c r="L24" s="149"/>
+      <c r="M24" s="149"/>
+      <c r="N24" s="149"/>
       <c r="O24" s="74">
         <f>COUNTIF($B$8:$B$120,"Jember")</f>
         <v>1</v>
@@ -8460,12 +8688,12 @@
         <v>182</v>
       </c>
       <c r="J25" s="28"/>
-      <c r="K25" s="135" t="s">
+      <c r="K25" s="148" t="s">
         <v>19</v>
       </c>
-      <c r="L25" s="136"/>
-      <c r="M25" s="136"/>
-      <c r="N25" s="136"/>
+      <c r="L25" s="149"/>
+      <c r="M25" s="149"/>
+      <c r="N25" s="149"/>
       <c r="O25" s="74">
         <f>COUNTIF($B$8:$B$120,"Kanreg 9 BKN Jayapura")</f>
         <v>1</v>
@@ -8519,12 +8747,12 @@
         <v>32</v>
       </c>
       <c r="J26" s="28"/>
-      <c r="K26" s="135" t="s">
+      <c r="K26" s="148" t="s">
         <v>23</v>
       </c>
-      <c r="L26" s="136"/>
-      <c r="M26" s="136"/>
-      <c r="N26" s="136"/>
+      <c r="L26" s="149"/>
+      <c r="M26" s="149"/>
+      <c r="N26" s="149"/>
       <c r="O26" s="74">
         <f>COUNTIF($B$8:$B$120,"LPP RRI Samarinda")</f>
         <v>2</v>
@@ -8578,12 +8806,12 @@
         <v>32</v>
       </c>
       <c r="J27" s="28"/>
-      <c r="K27" s="135" t="s">
+      <c r="K27" s="148" t="s">
         <v>16</v>
       </c>
-      <c r="L27" s="136"/>
-      <c r="M27" s="136"/>
-      <c r="N27" s="136"/>
+      <c r="L27" s="149"/>
+      <c r="M27" s="149"/>
+      <c r="N27" s="149"/>
       <c r="O27" s="74">
         <f>COUNTIF($B$8:$B$120,"Makassar 2")</f>
         <v>4</v>
@@ -8637,12 +8865,12 @@
         <v>32</v>
       </c>
       <c r="J28" s="28"/>
-      <c r="K28" s="135" t="s">
+      <c r="K28" s="148" t="s">
         <v>12</v>
       </c>
-      <c r="L28" s="136"/>
-      <c r="M28" s="136"/>
-      <c r="N28" s="136"/>
+      <c r="L28" s="149"/>
+      <c r="M28" s="149"/>
+      <c r="N28" s="149"/>
       <c r="O28" s="74">
         <f>COUNTIF($B$8:$B$120,"Palembang 2")</f>
         <v>4</v>
@@ -8696,12 +8924,12 @@
         <v>182</v>
       </c>
       <c r="J29" s="28"/>
-      <c r="K29" s="135" t="s">
+      <c r="K29" s="148" t="s">
         <v>21</v>
       </c>
-      <c r="L29" s="136"/>
-      <c r="M29" s="136"/>
-      <c r="N29" s="136"/>
+      <c r="L29" s="149"/>
+      <c r="M29" s="149"/>
+      <c r="N29" s="149"/>
       <c r="O29" s="74">
         <f>COUNTIF($B$8:$B$120,"Semarang 2")</f>
         <v>1</v>
@@ -8755,12 +8983,12 @@
         <v>32</v>
       </c>
       <c r="J30" s="28"/>
-      <c r="K30" s="156" t="s">
+      <c r="K30" s="169" t="s">
         <v>62</v>
       </c>
-      <c r="L30" s="157"/>
-      <c r="M30" s="157"/>
-      <c r="N30" s="157"/>
+      <c r="L30" s="170"/>
+      <c r="M30" s="170"/>
+      <c r="N30" s="170"/>
       <c r="O30" s="74">
         <f>COUNTIF($B$8:$B$120,"Pekanbaru 2")</f>
         <v>1</v>
@@ -8814,12 +9042,12 @@
         <v>32</v>
       </c>
       <c r="J31" s="28"/>
-      <c r="K31" s="137" t="s">
+      <c r="K31" s="150" t="s">
         <v>30</v>
       </c>
-      <c r="L31" s="138"/>
-      <c r="M31" s="138"/>
-      <c r="N31" s="138"/>
+      <c r="L31" s="151"/>
+      <c r="M31" s="151"/>
+      <c r="N31" s="151"/>
       <c r="O31" s="74">
         <f>COUNTIF($B$8:$B$120,"Serang")</f>
         <v>2</v>
@@ -8873,12 +9101,12 @@
         <v>182</v>
       </c>
       <c r="J32" s="28"/>
-      <c r="K32" s="137" t="s">
+      <c r="K32" s="150" t="s">
         <v>14</v>
       </c>
-      <c r="L32" s="138"/>
-      <c r="M32" s="138"/>
-      <c r="N32" s="138"/>
+      <c r="L32" s="151"/>
+      <c r="M32" s="151"/>
+      <c r="N32" s="151"/>
       <c r="O32" s="74">
         <f>COUNTIF($B$8:$B$120,"Surabaya 1")</f>
         <v>3</v>
@@ -8932,12 +9160,12 @@
         <v>32</v>
       </c>
       <c r="J33" s="28"/>
-      <c r="K33" s="137" t="s">
+      <c r="K33" s="150" t="s">
         <v>31</v>
       </c>
-      <c r="L33" s="138"/>
-      <c r="M33" s="138"/>
-      <c r="N33" s="138"/>
+      <c r="L33" s="151"/>
+      <c r="M33" s="151"/>
+      <c r="N33" s="151"/>
       <c r="O33" s="74">
         <f>COUNTIF($B$8:$B$120,"Tasikmalaya")</f>
         <v>1</v>
@@ -8991,12 +9219,12 @@
         <v>32</v>
       </c>
       <c r="J34" s="28"/>
-      <c r="K34" s="137" t="s">
+      <c r="K34" s="150" t="s">
         <v>26</v>
       </c>
-      <c r="L34" s="138"/>
-      <c r="M34" s="138"/>
-      <c r="N34" s="138"/>
+      <c r="L34" s="151"/>
+      <c r="M34" s="151"/>
+      <c r="N34" s="151"/>
       <c r="O34" s="74">
         <f>COUNTIF($B$8:$B$120,"UPT BKN Balikpapan")</f>
         <v>2</v>
@@ -9050,12 +9278,12 @@
         <v>32</v>
       </c>
       <c r="J35" s="28"/>
-      <c r="K35" s="137" t="s">
+      <c r="K35" s="150" t="s">
         <v>5</v>
       </c>
-      <c r="L35" s="138"/>
-      <c r="M35" s="138"/>
-      <c r="N35" s="138"/>
+      <c r="L35" s="151"/>
+      <c r="M35" s="151"/>
+      <c r="N35" s="151"/>
       <c r="O35" s="74">
         <f>COUNTIF($B$8:$B$120,"Yogyakarta 2")</f>
         <v>12</v>
@@ -9109,12 +9337,12 @@
         <v>32</v>
       </c>
       <c r="J36" s="28"/>
-      <c r="K36" s="137" t="s">
+      <c r="K36" s="150" t="s">
         <v>34</v>
       </c>
-      <c r="L36" s="138"/>
-      <c r="M36" s="138"/>
-      <c r="N36" s="138"/>
+      <c r="L36" s="151"/>
+      <c r="M36" s="151"/>
+      <c r="N36" s="151"/>
       <c r="O36" s="74">
         <f>COUNTIF($B$8:$B$120,"")</f>
         <v>3</v>
@@ -9168,12 +9396,12 @@
         <v>32</v>
       </c>
       <c r="J37" s="28"/>
-      <c r="K37" s="154" t="s">
+      <c r="K37" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="L37" s="155"/>
-      <c r="M37" s="155"/>
-      <c r="N37" s="155"/>
+      <c r="L37" s="168"/>
+      <c r="M37" s="168"/>
+      <c r="N37" s="168"/>
       <c r="O37" s="95">
         <f>SUM(O17:O36)</f>
         <v>113</v>
@@ -13332,12 +13560,12 @@
       <c r="AD120" s="12"/>
     </row>
     <row r="121" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="158" t="s">
-        <v>191</v>
-      </c>
-      <c r="B121" s="159"/>
-      <c r="C121" s="159"/>
-      <c r="D121" s="160"/>
+      <c r="A121" s="171" t="s">
+        <v>190</v>
+      </c>
+      <c r="B121" s="172"/>
+      <c r="C121" s="172"/>
+      <c r="D121" s="173"/>
       <c r="E121" s="88">
         <v>65</v>
       </c>
@@ -14723,22 +14951,22 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="144" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="134"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="M2" s="144"/>
+      <c r="N2" s="144"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -14753,20 +14981,20 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="134"/>
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
-      <c r="K3" s="134"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="134"/>
-      <c r="N3" s="134"/>
+      <c r="A3" s="144"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -14952,7 +15180,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="73"/>
       <c r="L8" s="70" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -15037,7 +15265,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="127"/>
       <c r="L10" s="71" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -21368,22 +21596,22 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="134" t="s">
+      <c r="A2" s="144" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="134"/>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="134"/>
+      <c r="B2" s="144"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="144"/>
+      <c r="E2" s="144"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
+      <c r="K2" s="144"/>
+      <c r="L2" s="144"/>
+      <c r="M2" s="144"/>
+      <c r="N2" s="144"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -21398,20 +21626,20 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="134"/>
-      <c r="B3" s="134"/>
-      <c r="C3" s="134"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-      <c r="H3" s="134"/>
-      <c r="I3" s="134"/>
-      <c r="J3" s="134"/>
-      <c r="K3" s="134"/>
-      <c r="L3" s="134"/>
-      <c r="M3" s="134"/>
-      <c r="N3" s="134"/>
+      <c r="A3" s="144"/>
+      <c r="B3" s="144"/>
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -21595,7 +21823,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="73"/>
       <c r="L8" s="70" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -21691,7 +21919,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="127"/>
       <c r="L10" s="71" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -27712,18 +27940,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="165" t="s">
-        <v>199</v>
-      </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
+      <c r="A1" s="174" t="s">
+        <v>198</v>
+      </c>
+      <c r="B1" s="174"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="138"/>
+      <c r="E1" s="138"/>
+      <c r="F1" s="138"/>
+      <c r="G1" s="138"/>
+      <c r="H1" s="138"/>
+      <c r="I1" s="138"/>
+      <c r="J1" s="138"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -27742,16 +27970,16 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="165"/>
-      <c r="B2" s="165"/>
-      <c r="C2" s="165"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="166"/>
-      <c r="I2" s="166"/>
-      <c r="J2" s="166"/>
+      <c r="A2" s="174"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -27770,8 +27998,8 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="167" t="s">
-        <v>204</v>
+      <c r="A3" s="139" t="s">
+        <v>203</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -27800,8 +28028,8 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="168" t="s">
-        <v>200</v>
+      <c r="A4" s="140" t="s">
+        <v>199</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -27859,7 +28087,7 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -27888,8 +28116,8 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" s="164" t="s">
-        <v>201</v>
+      <c r="A7" s="137" t="s">
+        <v>200</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -27947,7 +28175,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -27976,8 +28204,8 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="164" t="s">
-        <v>202</v>
+      <c r="A10" s="137" t="s">
+        <v>201</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -28035,7 +28263,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -28064,8 +28292,8 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="164" t="s">
-        <v>203</v>
+      <c r="A13" s="137" t="s">
+        <v>211</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -28094,7 +28322,7 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="169"/>
+      <c r="A14" s="141"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -28122,7 +28350,9 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="169"/>
+      <c r="A15" s="15" t="s">
+        <v>206</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -28150,7 +28380,9 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="169"/>
+      <c r="A16" s="137" t="s">
+        <v>202</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -28178,7 +28410,7 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="169"/>
+      <c r="A17" s="141"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -30537,9 +30769,11 @@
     <hyperlink ref="A4" r:id="rId1" xr:uid="{418F9254-726D-48FE-ABFE-EDBD76CE0CEB}"/>
     <hyperlink ref="A7" r:id="rId2" xr:uid="{E7EDFE02-E3B0-4473-8FF5-8FBEA8607365}"/>
     <hyperlink ref="A10" r:id="rId3" xr:uid="{4F7A6C5C-FA31-41E7-B6E3-D9A554227A59}"/>
-    <hyperlink ref="A13" r:id="rId4" xr:uid="{FBF40374-2AF9-401D-B8EA-5B09270F18EC}"/>
+    <hyperlink ref="A16" r:id="rId4" xr:uid="{FBF40374-2AF9-401D-B8EA-5B09270F18EC}"/>
+    <hyperlink ref="A13" r:id="rId5" xr:uid="{34A332A0-69FE-4C98-800F-69DF578A0047}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -30554,18 +30788,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="161" t="s">
-        <v>196</v>
-      </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
-      <c r="F1" s="162"/>
-      <c r="G1" s="162"/>
-      <c r="H1" s="162"/>
-      <c r="I1" s="162"/>
-      <c r="J1" s="162"/>
+      <c r="A1" s="134" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="H1" s="135"/>
+      <c r="I1" s="135"/>
+      <c r="J1" s="135"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -30584,18 +30818,18 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="163" t="s">
-        <v>195</v>
-      </c>
-      <c r="B2" s="162"/>
-      <c r="C2" s="162"/>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
+      <c r="A2" s="136" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" s="135"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -30643,7 +30877,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -30672,8 +30906,8 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="164" t="s">
-        <v>198</v>
+      <c r="A5" s="137" t="s">
+        <v>197</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>

</xml_diff>